<commit_message>
Add SubscriptionStatus example (and cleanup)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQ-subscription-status.xlsx
+++ b/output/StructureDefinition-CEQ-subscription-status.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$48</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="135">
   <si>
     <t>Path</t>
   </si>
@@ -247,7 +247,7 @@
     <t>Parameters.parameter</t>
   </si>
   <si>
-    <t>4</t>
+    <t>3</t>
   </si>
   <si>
     <t xml:space="preserve">BackboneElement
@@ -425,10 +425,10 @@
     <t>status</t>
   </si>
   <si>
+    <t>valueCode</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/subscription-status</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
   <si>
     <t>subscriptionEventCount</t>
@@ -587,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK55"/>
+  <dimension ref="A1:AK48"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -4401,7 +4401,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
         <v>105</v>
       </c>
@@ -4459,26 +4459,26 @@
         <v>38</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="X37" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y37" t="s" s="2">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AB37" s="2"/>
       <c r="AC37" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD37" t="s" s="2">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="AE37" t="s" s="2">
         <v>105</v>
@@ -4504,9 +4504,11 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="B38" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="C38" t="s" s="2">
         <v>38</v>
       </c>
@@ -4527,17 +4529,15 @@
         <v>47</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>38</v>
@@ -4562,13 +4562,11 @@
         <v>38</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="X38" s="2"/>
       <c r="Y38" t="s" s="2">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>38</v>
@@ -4586,7 +4584,7 @@
         <v>38</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>39</v>
@@ -4598,7 +4596,7 @@
         <v>109</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>38</v>
@@ -4609,7 +4607,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -4620,7 +4618,7 @@
         <v>39</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>38</v>
@@ -4632,16 +4630,16 @@
         <v>47</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -4691,46 +4689,44 @@
         <v>38</v>
       </c>
       <c r="AE39" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK39" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" hidden="true">
+      <c r="A40" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="AF39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>131</v>
-      </c>
+      <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>38</v>
@@ -4739,15 +4735,17 @@
         <v>47</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="M40" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>118</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>38</v>
@@ -4796,7 +4794,7 @@
         <v>38</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>39</v>
@@ -4808,7 +4806,7 @@
         <v>38</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>38</v>
@@ -4817,38 +4815,40 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="B41" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>132</v>
+      </c>
       <c r="C41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>46</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -4899,41 +4899,41 @@
         <v>38</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>38</v>
@@ -4945,17 +4945,15 @@
         <v>38</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>92</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>38</v>
@@ -5004,19 +5002,19 @@
         <v>38</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>38</v>
@@ -5027,11 +5025,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -5044,26 +5042,24 @@
         <v>38</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J43" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="M43" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="N43" t="s" s="2">
-        <v>99</v>
-      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>38</v>
       </c>
@@ -5111,7 +5107,7 @@
         <v>38</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>39</v>
@@ -5129,44 +5125,48 @@
         <v>38</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I44" t="s" s="2">
         <v>47</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>38</v>
       </c>
@@ -5214,30 +5214,30 @@
         <v>38</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F45" t="s" s="2">
         <v>46</v>
@@ -5260,13 +5260,13 @@
         <v>47</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -5275,7 +5275,7 @@
       </c>
       <c r="P45" s="2"/>
       <c r="Q45" t="s" s="2">
-        <v>38</v>
+        <v>133</v>
       </c>
       <c r="R45" t="s" s="2">
         <v>38</v>
@@ -5317,16 +5317,16 @@
         <v>38</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>46</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>58</v>
@@ -5338,9 +5338,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" hidden="true">
+    <row r="46">
       <c r="A46" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -5348,13 +5348,13 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F46" t="s" s="2">
         <v>46</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>38</v>
@@ -5363,17 +5363,15 @@
         <v>47</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>38</v>
@@ -5422,7 +5420,7 @@
         <v>38</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>39</v>
@@ -5434,7 +5432,7 @@
         <v>109</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>38</v>
@@ -5445,7 +5443,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -5456,7 +5454,7 @@
         <v>39</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>38</v>
@@ -5468,16 +5466,16 @@
         <v>47</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -5527,46 +5525,44 @@
         <v>38</v>
       </c>
       <c r="AE47" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" hidden="true">
+      <c r="A48" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="AF47" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH47" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI47" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AJ47" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>132</v>
-      </c>
+      <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>38</v>
@@ -5575,15 +5571,17 @@
         <v>47</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="M48" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>118</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>38</v>
@@ -5632,7 +5630,7 @@
         <v>38</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>39</v>
@@ -5644,748 +5642,17 @@
         <v>38</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" hidden="true">
-      <c r="A49" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F49" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="J49" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="K49" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P49" s="2"/>
-      <c r="Q49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AF49" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG49" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AJ49" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK49" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" hidden="true">
-      <c r="A50" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="J50" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="N50" s="2"/>
-      <c r="O50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" hidden="true">
-      <c r="A51" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H51" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="I51" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="J51" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" hidden="true">
-      <c r="A52" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="F52" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I52" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="J52" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="K52" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="R52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="F53" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G53" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="H53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I53" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="J53" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="K53" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P53" s="2"/>
-      <c r="Q53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="N54" s="2"/>
-      <c r="O54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" hidden="true">
-      <c r="A55" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="N55" s="2"/>
-      <c r="O55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK55" t="s" s="2">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK55">
+  <autoFilter ref="A1:AK48">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6395,7 +5662,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI54">
+  <conditionalFormatting sqref="A2:AI47">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>